<commit_message>
Updated with the changes of page and test classes.
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\repository2\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBBCE8E-2674-4FDD-A285-5226CB93F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020F156-6495-4A60-AF13-53E71A00A9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37260D1C-802F-49EC-B1AB-AA4A214E8944}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Vishnu</t>
-  </si>
-  <si>
     <t>Larry</t>
   </si>
   <si>
@@ -39,7 +36,10 @@
     <t>Ayaansh</t>
   </si>
   <si>
-    <t>Appu</t>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Mary</t>
   </si>
 </sst>
 </file>
@@ -401,19 +401,19 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -423,7 +423,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated with latest modifications.
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\repository2\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020F156-6495-4A60-AF13-53E71A00A9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64553D90-92FE-4CC9-8378-180392B7C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37260D1C-802F-49EC-B1AB-AA4A214E8944}"/>
   </bookViews>
@@ -33,13 +33,13 @@
     <t>Menon</t>
   </si>
   <si>
-    <t>Ayaansh</t>
-  </si>
-  <si>
     <t>Leonardo</t>
   </si>
   <si>
     <t>Mary</t>
+  </si>
+  <si>
+    <t>Janaki</t>
   </si>
 </sst>
 </file>
@@ -400,15 +400,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED73A0EE-58B8-4E2C-AAC7-1A86B4991FAB}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -418,7 +416,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -428,7 +426,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with the new changes.
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\repository2\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64553D90-92FE-4CC9-8378-180392B7C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0F9650-DEA2-4FFD-A0EA-A27C21848869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37260D1C-802F-49EC-B1AB-AA4A214E8944}"/>
   </bookViews>
@@ -36,10 +36,10 @@
     <t>Leonardo</t>
   </si>
   <si>
-    <t>Mary</t>
+    <t>Manu</t>
   </si>
   <si>
-    <t>Janaki</t>
+    <t>Ishaan</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated with latest changes...
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/AdminUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\repository2\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C059368-20F6-4366-8A93-DB5DF8BC44F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFECC6E-5BF8-407A-A289-884E91BD9520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37260D1C-802F-49EC-B1AB-AA4A214E8944}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Larry</t>
   </si>
   <si>
-    <t>Leonardo</t>
-  </si>
-  <si>
     <t>Manu</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>Appu</t>
+  </si>
+  <si>
+    <t>Annie</t>
   </si>
 </sst>
 </file>
@@ -401,14 +401,14 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -418,17 +418,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>